<commit_message>
Disabling the buttons before login
</commit_message>
<xml_diff>
--- a/WebsiteData.xlsx
+++ b/WebsiteData.xlsx
@@ -1,31 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\OneDrive - Nile University\Desktop\TaskManagerWebsite\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013026E2-3FC0-4E14-B248-AB9F6BACEA76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
-    <sheet name="User Data" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="User Data" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Registration Counter</t>
   </si>
@@ -43,19 +32,28 @@
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>Julia</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -359,16 +357,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
-    </sheetView>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.3" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -386,6 +382,26 @@
       </c>
       <c r="F1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding comments in the TaskFile
</commit_message>
<xml_diff>
--- a/WebsiteData.xlsx
+++ b/WebsiteData.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CB1E02-423C-430E-9880-30F14A46B7AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
-    <sheet name="User Data" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="User Data" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Registration Counter</t>
   </si>
@@ -33,19 +32,31 @@
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>0100</t>
+  </si>
+  <si>
+    <t>test@gmail.com</t>
+  </si>
+  <si>
+    <t>test123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -68,8 +79,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -349,14 +361,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="305" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0" zoomScale="135" zoomScaleNormal="100">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.3" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" customWidth="1"/>
+    <col min="6" max="6" width="8.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -368,7 +388,7 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -378,7 +398,26 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>